<commit_message>
updated prelim design report
</commit_message>
<xml_diff>
--- a/reports/existing solutions analysis.xlsx
+++ b/reports/existing solutions analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\m3dd\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\FSERV\home\jb7008\Desktop\m3dd\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336801A3-AD7B-48B9-84FB-5A5CB37A7F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479DC4D9-ADE3-43B6-B75B-9E0DDDB0E48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C1DFBB7-4E11-441D-8ED7-B862C9D4336F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C1DFBB7-4E11-441D-8ED7-B862C9D4336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,16 +637,16 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,7 +666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -699,7 +699,7 @@
         <v>17576000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -732,7 +732,7 @@
         <v>31360000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -765,7 +765,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -798,7 +798,7 @@
         <v>4766250</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -831,7 +831,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -864,7 +864,7 @@
         <v>16500000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -897,7 +897,7 @@
         <v>27000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -930,7 +930,7 @@
         <v>207000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -963,7 +963,7 @@
         <v>26520000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -996,7 +996,7 @@
         <v>10692000</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>58516780</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>129600000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>SUM(C2:C13)/12</f>
         <v>491.66666666666669</v>
@@ -1084,7 +1084,7 @@
         <v>50127585.833333336</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
@@ -1117,8 +1117,8 @@
         <v>111720000</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:13" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>38</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>45</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13.919999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>39</v>
       </c>
@@ -1190,21 +1190,21 @@
         <v>24</v>
       </c>
       <c r="C24" s="12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D24" s="12">
         <v>1</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M24" s="12">
         <f>B24*C24</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9.6000000000000014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>40</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>49.92</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>41</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>5.1929999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>42</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>43</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>44</v>
       </c>
@@ -1336,24 +1336,24 @@
         <v>98.399999999999991</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="M31" s="12"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>48</v>
       </c>
       <c r="E32">
         <f>SUM(E22:E30)</f>
-        <v>17.326000000000001</v>
+        <v>17.225999999999999</v>
       </c>
       <c r="F32">
         <f>SUM(E22:E29)</f>
-        <v>13.225999999999999</v>
+        <v>13.126000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>